<commit_message>
fix storage type typo
</commit_message>
<xml_diff>
--- a/inputs/parzen-energy-storage-database.xlsx
+++ b/inputs/parzen-energy-storage-database.xlsx
@@ -466,16 +466,16 @@
     <t xml:space="preserve">p.111 (p.133)</t>
   </si>
   <si>
+    <t xml:space="preserve">elec-phes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phes-elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pumped-Heat</t>
+  </si>
+  <si>
     <t xml:space="preserve">thermal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elec-phes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phes-elec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pumped-Heat</t>
   </si>
   <si>
     <t xml:space="preserve">phes</t>
@@ -758,8 +758,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B180" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F229" activeCellId="0" sqref="F229:J229"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A269" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A327" activeCellId="0" sqref="A327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12850,10 +12850,10 @@
         <v>131</v>
       </c>
       <c r="B327" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C327" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C327" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D327" s="0" t="s">
         <v>29</v>
@@ -12886,10 +12886,10 @@
         <v>131</v>
       </c>
       <c r="B328" s="0" t="s">
-        <v>148</v>
+        <v>13</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D328" s="0" t="s">
         <v>29</v>
@@ -13096,10 +13096,10 @@
     </row>
     <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B334" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B334" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="C334" s="0" t="s">
         <v>152</v>
@@ -13134,10 +13134,10 @@
     </row>
     <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B335" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B335" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="C335" s="0" t="s">
         <v>142</v>
@@ -13172,13 +13172,13 @@
     </row>
     <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B336" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B336" s="0" t="s">
+      <c r="C336" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C336" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D336" s="0" t="s">
         <v>15</v>
@@ -13211,13 +13211,13 @@
     </row>
     <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B337" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B337" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C337" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D337" s="0" t="s">
         <v>15</v>
@@ -13247,10 +13247,10 @@
     </row>
     <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B338" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B338" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D338" s="0" t="s">
         <v>15</v>
@@ -13282,10 +13282,10 @@
     </row>
     <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B339" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B339" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D339" s="0" t="s">
         <v>15</v>
@@ -13318,10 +13318,10 @@
     </row>
     <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B340" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B340" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D340" s="0" t="s">
         <v>15</v>
@@ -13354,10 +13354,10 @@
     </row>
     <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B341" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B341" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D341" s="0" t="s">
         <v>29</v>
@@ -13390,10 +13390,10 @@
     </row>
     <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B342" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B342" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D342" s="0" t="s">
         <v>29</v>
@@ -13426,13 +13426,13 @@
     </row>
     <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B343" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B343" s="0" t="s">
+      <c r="C343" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C343" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D343" s="0" t="s">
         <v>29</v>
@@ -13462,13 +13462,13 @@
     </row>
     <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B344" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B344" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C344" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D344" s="0" t="s">
         <v>29</v>
@@ -13498,13 +13498,13 @@
     </row>
     <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B345" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B345" s="0" t="s">
+      <c r="C345" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C345" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D345" s="0" t="s">
         <v>36</v>
@@ -13530,13 +13530,13 @@
     </row>
     <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B346" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B346" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C346" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D346" s="0" t="s">
         <v>36</v>
@@ -13566,13 +13566,13 @@
     </row>
     <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B347" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B347" s="0" t="s">
+      <c r="C347" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C347" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D347" s="0" t="s">
         <v>38</v>
@@ -13601,13 +13601,13 @@
     </row>
     <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B348" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B348" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C348" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D348" s="0" t="s">
         <v>38</v>
@@ -13636,10 +13636,10 @@
     </row>
     <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B349" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B349" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="C349" s="0" t="s">
         <v>152</v>
@@ -13671,10 +13671,10 @@
     </row>
     <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B350" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B350" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="C350" s="0" t="s">
         <v>152</v>
@@ -13709,10 +13709,10 @@
     </row>
     <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B351" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B351" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="C351" s="0" t="s">
         <v>142</v>
@@ -13747,13 +13747,13 @@
     </row>
     <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B352" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B352" s="0" t="s">
+      <c r="C352" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C352" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D352" s="0" t="s">
         <v>15</v>
@@ -13786,13 +13786,13 @@
     </row>
     <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B353" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B353" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C353" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D353" s="0" t="s">
         <v>15</v>
@@ -13822,10 +13822,10 @@
     </row>
     <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B354" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B354" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D354" s="0" t="s">
         <v>15</v>
@@ -13857,10 +13857,10 @@
     </row>
     <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B355" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B355" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D355" s="0" t="s">
         <v>15</v>
@@ -13893,10 +13893,10 @@
     </row>
     <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B356" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B356" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D356" s="0" t="s">
         <v>15</v>
@@ -13929,10 +13929,10 @@
     </row>
     <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B357" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B357" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="D357" s="0" t="s">
         <v>29</v>
@@ -13965,10 +13965,10 @@
     </row>
     <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B358" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B358" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="C358" s="0" t="s">
         <v>142</v>
@@ -14004,13 +14004,13 @@
     </row>
     <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B359" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B359" s="0" t="s">
+      <c r="C359" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C359" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D359" s="0" t="s">
         <v>29</v>
@@ -14040,13 +14040,13 @@
     </row>
     <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B360" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B360" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C360" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D360" s="0" t="s">
         <v>29</v>
@@ -14076,13 +14076,13 @@
     </row>
     <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B361" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B361" s="0" t="s">
+      <c r="C361" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C361" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D361" s="0" t="s">
         <v>36</v>
@@ -14108,13 +14108,13 @@
     </row>
     <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B362" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B362" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C362" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D362" s="0" t="s">
         <v>36</v>
@@ -14144,13 +14144,13 @@
     </row>
     <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B363" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B363" s="0" t="s">
+      <c r="C363" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C363" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="D363" s="0" t="s">
         <v>38</v>
@@ -14179,13 +14179,13 @@
     </row>
     <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B364" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B364" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C364" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D364" s="0" t="s">
         <v>38</v>
@@ -14214,10 +14214,10 @@
     </row>
     <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B365" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B365" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="C365" s="0" t="s">
         <v>152</v>
@@ -14252,7 +14252,7 @@
         <v>168</v>
       </c>
       <c r="B366" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C366" s="0" t="s">
         <v>169</v>
@@ -14290,7 +14290,7 @@
         <v>168</v>
       </c>
       <c r="B367" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C367" s="0" t="s">
         <v>142</v>
@@ -14328,7 +14328,7 @@
         <v>168</v>
       </c>
       <c r="B368" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C368" s="0" t="s">
         <v>172</v>
@@ -14367,7 +14367,7 @@
         <v>168</v>
       </c>
       <c r="B369" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C369" s="0" t="s">
         <v>173</v>
@@ -14403,7 +14403,7 @@
         <v>168</v>
       </c>
       <c r="B370" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D370" s="0" t="s">
         <v>15</v>
@@ -14438,7 +14438,7 @@
         <v>168</v>
       </c>
       <c r="B371" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D371" s="0" t="s">
         <v>15</v>
@@ -14473,7 +14473,7 @@
         <v>168</v>
       </c>
       <c r="B372" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D372" s="0" t="s">
         <v>15</v>
@@ -14508,7 +14508,7 @@
         <v>168</v>
       </c>
       <c r="B373" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D373" s="0" t="s">
         <v>29</v>
@@ -14544,7 +14544,7 @@
         <v>168</v>
       </c>
       <c r="B374" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C374" s="0" t="s">
         <v>142</v>
@@ -14583,7 +14583,7 @@
         <v>168</v>
       </c>
       <c r="B375" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C375" s="0" t="s">
         <v>172</v>
@@ -14619,7 +14619,7 @@
         <v>168</v>
       </c>
       <c r="B376" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C376" s="0" t="s">
         <v>173</v>
@@ -14655,7 +14655,7 @@
         <v>168</v>
       </c>
       <c r="B377" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C377" s="0" t="s">
         <v>172</v>
@@ -14685,7 +14685,7 @@
         <v>168</v>
       </c>
       <c r="B378" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C378" s="0" t="s">
         <v>173</v>
@@ -14721,7 +14721,7 @@
         <v>168</v>
       </c>
       <c r="B379" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C379" s="0" t="s">
         <v>172</v>
@@ -14756,7 +14756,7 @@
         <v>168</v>
       </c>
       <c r="B380" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C380" s="0" t="s">
         <v>173</v>
@@ -14791,7 +14791,7 @@
         <v>168</v>
       </c>
       <c r="B381" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C381" s="0" t="s">
         <v>169</v>
@@ -14826,7 +14826,7 @@
         <v>168</v>
       </c>
       <c r="B382" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C382" s="0" t="s">
         <v>169</v>
@@ -14864,7 +14864,7 @@
         <v>168</v>
       </c>
       <c r="B383" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C383" s="0" t="s">
         <v>142</v>
@@ -14902,7 +14902,7 @@
         <v>168</v>
       </c>
       <c r="B384" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C384" s="0" t="s">
         <v>172</v>
@@ -14941,7 +14941,7 @@
         <v>168</v>
       </c>
       <c r="B385" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C385" s="0" t="s">
         <v>173</v>
@@ -14977,7 +14977,7 @@
         <v>168</v>
       </c>
       <c r="B386" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D386" s="0" t="s">
         <v>15</v>
@@ -15012,7 +15012,7 @@
         <v>168</v>
       </c>
       <c r="B387" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D387" s="0" t="s">
         <v>15</v>
@@ -15047,7 +15047,7 @@
         <v>168</v>
       </c>
       <c r="B388" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D388" s="0" t="s">
         <v>15</v>
@@ -15082,7 +15082,7 @@
         <v>168</v>
       </c>
       <c r="B389" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D389" s="0" t="s">
         <v>29</v>
@@ -15118,7 +15118,7 @@
         <v>168</v>
       </c>
       <c r="B390" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C390" s="0" t="s">
         <v>142</v>
@@ -15157,7 +15157,7 @@
         <v>168</v>
       </c>
       <c r="B391" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C391" s="0" t="s">
         <v>172</v>
@@ -15193,7 +15193,7 @@
         <v>168</v>
       </c>
       <c r="B392" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C392" s="0" t="s">
         <v>173</v>
@@ -15229,7 +15229,7 @@
         <v>168</v>
       </c>
       <c r="B393" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C393" s="0" t="s">
         <v>172</v>
@@ -15264,7 +15264,7 @@
         <v>168</v>
       </c>
       <c r="B394" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C394" s="0" t="s">
         <v>173</v>
@@ -15297,7 +15297,7 @@
         <v>168</v>
       </c>
       <c r="B395" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C395" s="0" t="s">
         <v>172</v>
@@ -15332,7 +15332,7 @@
         <v>168</v>
       </c>
       <c r="B396" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C396" s="0" t="s">
         <v>173</v>
@@ -15367,7 +15367,7 @@
         <v>168</v>
       </c>
       <c r="B397" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C397" s="0" t="s">
         <v>169</v>
@@ -15402,7 +15402,7 @@
         <v>177</v>
       </c>
       <c r="B398" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C398" s="0" t="s">
         <v>178</v>
@@ -15441,7 +15441,7 @@
         <v>177</v>
       </c>
       <c r="B399" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C399" s="0" t="s">
         <v>142</v>
@@ -15480,7 +15480,7 @@
         <v>177</v>
       </c>
       <c r="B400" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C400" s="0" t="s">
         <v>182</v>
@@ -15513,7 +15513,7 @@
         <v>177</v>
       </c>
       <c r="B401" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C401" s="0" t="s">
         <v>184</v>
@@ -15546,7 +15546,7 @@
         <v>177</v>
       </c>
       <c r="B402" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D402" s="0" t="s">
         <v>15</v>
@@ -15582,7 +15582,7 @@
         <v>177</v>
       </c>
       <c r="B403" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D403" s="0" t="s">
         <v>29</v>
@@ -15618,7 +15618,7 @@
         <v>177</v>
       </c>
       <c r="B404" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C404" s="0" t="s">
         <v>142</v>
@@ -15657,7 +15657,7 @@
         <v>177</v>
       </c>
       <c r="B405" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C405" s="0" t="s">
         <v>182</v>
@@ -15693,7 +15693,7 @@
         <v>177</v>
       </c>
       <c r="B406" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C406" s="0" t="s">
         <v>184</v>
@@ -15729,7 +15729,7 @@
         <v>177</v>
       </c>
       <c r="B407" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C407" s="0" t="s">
         <v>184</v>
@@ -15765,7 +15765,7 @@
         <v>177</v>
       </c>
       <c r="B408" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C408" s="0" t="s">
         <v>182</v>
@@ -15800,7 +15800,7 @@
         <v>177</v>
       </c>
       <c r="B409" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C409" s="0" t="s">
         <v>184</v>
@@ -15835,7 +15835,7 @@
         <v>177</v>
       </c>
       <c r="B410" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C410" s="0" t="s">
         <v>182</v>
@@ -15870,7 +15870,7 @@
         <v>177</v>
       </c>
       <c r="B411" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C411" s="0" t="s">
         <v>178</v>
@@ -15905,7 +15905,7 @@
         <v>177</v>
       </c>
       <c r="B412" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C412" s="0" t="s">
         <v>178</v>
@@ -15943,7 +15943,7 @@
         <v>177</v>
       </c>
       <c r="B413" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C413" s="0" t="s">
         <v>142</v>
@@ -15981,7 +15981,7 @@
         <v>177</v>
       </c>
       <c r="B414" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C414" s="0" t="s">
         <v>182</v>
@@ -16014,7 +16014,7 @@
         <v>177</v>
       </c>
       <c r="B415" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C415" s="0" t="s">
         <v>184</v>
@@ -16047,7 +16047,7 @@
         <v>177</v>
       </c>
       <c r="B416" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D416" s="0" t="s">
         <v>15</v>
@@ -16083,7 +16083,7 @@
         <v>177</v>
       </c>
       <c r="B417" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D417" s="0" t="s">
         <v>29</v>
@@ -16119,7 +16119,7 @@
         <v>177</v>
       </c>
       <c r="B418" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C418" s="0" t="s">
         <v>142</v>
@@ -16158,7 +16158,7 @@
         <v>177</v>
       </c>
       <c r="B419" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C419" s="0" t="s">
         <v>182</v>
@@ -16194,7 +16194,7 @@
         <v>177</v>
       </c>
       <c r="B420" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C420" s="0" t="s">
         <v>184</v>
@@ -16230,7 +16230,7 @@
         <v>177</v>
       </c>
       <c r="B421" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C421" s="0" t="s">
         <v>184</v>
@@ -16266,7 +16266,7 @@
         <v>177</v>
       </c>
       <c r="B422" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C422" s="0" t="s">
         <v>182</v>
@@ -16301,7 +16301,7 @@
         <v>177</v>
       </c>
       <c r="B423" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C423" s="0" t="s">
         <v>184</v>
@@ -16336,7 +16336,7 @@
         <v>177</v>
       </c>
       <c r="B424" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C424" s="0" t="s">
         <v>182</v>
@@ -16371,7 +16371,7 @@
         <v>177</v>
       </c>
       <c r="B425" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C425" s="0" t="s">
         <v>178</v>
@@ -16406,7 +16406,7 @@
         <v>189</v>
       </c>
       <c r="B426" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C426" s="0" t="s">
         <v>190</v>
@@ -16445,7 +16445,7 @@
         <v>189</v>
       </c>
       <c r="B427" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C427" s="0" t="s">
         <v>142</v>
@@ -16484,7 +16484,7 @@
         <v>189</v>
       </c>
       <c r="B428" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C428" s="0" t="s">
         <v>191</v>
@@ -16517,7 +16517,7 @@
         <v>189</v>
       </c>
       <c r="B429" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C429" s="0" t="s">
         <v>192</v>
@@ -16550,7 +16550,7 @@
         <v>189</v>
       </c>
       <c r="B430" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D430" s="0" t="s">
         <v>15</v>
@@ -16586,7 +16586,7 @@
         <v>189</v>
       </c>
       <c r="B431" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D431" s="0" t="s">
         <v>29</v>
@@ -16622,7 +16622,7 @@
         <v>189</v>
       </c>
       <c r="B432" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C432" s="0" t="s">
         <v>142</v>
@@ -16661,7 +16661,7 @@
         <v>189</v>
       </c>
       <c r="B433" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C433" s="0" t="s">
         <v>191</v>
@@ -16697,7 +16697,7 @@
         <v>189</v>
       </c>
       <c r="B434" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C434" s="0" t="s">
         <v>192</v>
@@ -16733,7 +16733,7 @@
         <v>189</v>
       </c>
       <c r="B435" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C435" s="0" t="s">
         <v>192</v>
@@ -16769,7 +16769,7 @@
         <v>189</v>
       </c>
       <c r="B436" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C436" s="0" t="s">
         <v>191</v>
@@ -16805,7 +16805,7 @@
         <v>189</v>
       </c>
       <c r="B437" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C437" s="0" t="s">
         <v>192</v>
@@ -16840,7 +16840,7 @@
         <v>189</v>
       </c>
       <c r="B438" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C438" s="0" t="s">
         <v>191</v>
@@ -16875,7 +16875,7 @@
         <v>189</v>
       </c>
       <c r="B439" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C439" s="0" t="s">
         <v>190</v>
@@ -16910,7 +16910,7 @@
         <v>189</v>
       </c>
       <c r="B440" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C440" s="0" t="s">
         <v>190</v>
@@ -16948,7 +16948,7 @@
         <v>189</v>
       </c>
       <c r="B441" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C441" s="0" t="s">
         <v>142</v>
@@ -16986,7 +16986,7 @@
         <v>189</v>
       </c>
       <c r="B442" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C442" s="0" t="s">
         <v>191</v>
@@ -17019,7 +17019,7 @@
         <v>189</v>
       </c>
       <c r="B443" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C443" s="0" t="s">
         <v>192</v>
@@ -17052,7 +17052,7 @@
         <v>189</v>
       </c>
       <c r="B444" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D444" s="0" t="s">
         <v>15</v>
@@ -17088,7 +17088,7 @@
         <v>189</v>
       </c>
       <c r="B445" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D445" s="0" t="s">
         <v>29</v>
@@ -17124,7 +17124,7 @@
         <v>189</v>
       </c>
       <c r="B446" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C446" s="0" t="s">
         <v>142</v>
@@ -17163,7 +17163,7 @@
         <v>189</v>
       </c>
       <c r="B447" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C447" s="0" t="s">
         <v>191</v>
@@ -17199,7 +17199,7 @@
         <v>189</v>
       </c>
       <c r="B448" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C448" s="0" t="s">
         <v>192</v>
@@ -17235,7 +17235,7 @@
         <v>189</v>
       </c>
       <c r="B449" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C449" s="0" t="s">
         <v>192</v>
@@ -17271,7 +17271,7 @@
         <v>189</v>
       </c>
       <c r="B450" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C450" s="0" t="s">
         <v>191</v>
@@ -17307,7 +17307,7 @@
         <v>189</v>
       </c>
       <c r="B451" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C451" s="0" t="s">
         <v>192</v>
@@ -17342,7 +17342,7 @@
         <v>189</v>
       </c>
       <c r="B452" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C452" s="0" t="s">
         <v>191</v>
@@ -17377,7 +17377,7 @@
         <v>189</v>
       </c>
       <c r="B453" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C453" s="0" t="s">
         <v>190</v>
@@ -17412,7 +17412,7 @@
         <v>193</v>
       </c>
       <c r="B454" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C454" s="0" t="s">
         <v>194</v>
@@ -17451,7 +17451,7 @@
         <v>193</v>
       </c>
       <c r="B455" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C455" s="0" t="s">
         <v>142</v>
@@ -17490,7 +17490,7 @@
         <v>193</v>
       </c>
       <c r="B456" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C456" s="0" t="s">
         <v>195</v>
@@ -17523,7 +17523,7 @@
         <v>193</v>
       </c>
       <c r="B457" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C457" s="0" t="s">
         <v>196</v>
@@ -17556,7 +17556,7 @@
         <v>193</v>
       </c>
       <c r="B458" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D458" s="0" t="s">
         <v>15</v>
@@ -17592,7 +17592,7 @@
         <v>193</v>
       </c>
       <c r="B459" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D459" s="0" t="s">
         <v>29</v>
@@ -17628,7 +17628,7 @@
         <v>193</v>
       </c>
       <c r="B460" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C460" s="0" t="s">
         <v>142</v>
@@ -17667,7 +17667,7 @@
         <v>193</v>
       </c>
       <c r="B461" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C461" s="0" t="s">
         <v>195</v>
@@ -17703,7 +17703,7 @@
         <v>193</v>
       </c>
       <c r="B462" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C462" s="0" t="s">
         <v>196</v>
@@ -17739,7 +17739,7 @@
         <v>193</v>
       </c>
       <c r="B463" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C463" s="0" t="s">
         <v>196</v>
@@ -17775,7 +17775,7 @@
         <v>193</v>
       </c>
       <c r="B464" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C464" s="0" t="s">
         <v>195</v>
@@ -17811,7 +17811,7 @@
         <v>193</v>
       </c>
       <c r="B465" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C465" s="0" t="s">
         <v>196</v>
@@ -17846,7 +17846,7 @@
         <v>193</v>
       </c>
       <c r="B466" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C466" s="0" t="s">
         <v>195</v>
@@ -17881,7 +17881,7 @@
         <v>193</v>
       </c>
       <c r="B467" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C467" s="0" t="s">
         <v>194</v>
@@ -17916,7 +17916,7 @@
         <v>193</v>
       </c>
       <c r="B468" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C468" s="0" t="s">
         <v>194</v>
@@ -17954,7 +17954,7 @@
         <v>193</v>
       </c>
       <c r="B469" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C469" s="0" t="s">
         <v>142</v>
@@ -17992,7 +17992,7 @@
         <v>193</v>
       </c>
       <c r="B470" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C470" s="0" t="s">
         <v>195</v>
@@ -18025,7 +18025,7 @@
         <v>193</v>
       </c>
       <c r="B471" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C471" s="0" t="s">
         <v>196</v>
@@ -18058,7 +18058,7 @@
         <v>193</v>
       </c>
       <c r="B472" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D472" s="0" t="s">
         <v>15</v>
@@ -18094,7 +18094,7 @@
         <v>193</v>
       </c>
       <c r="B473" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D473" s="0" t="s">
         <v>29</v>
@@ -18130,7 +18130,7 @@
         <v>193</v>
       </c>
       <c r="B474" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C474" s="0" t="s">
         <v>142</v>
@@ -18169,7 +18169,7 @@
         <v>193</v>
       </c>
       <c r="B475" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C475" s="0" t="s">
         <v>195</v>
@@ -18205,7 +18205,7 @@
         <v>193</v>
       </c>
       <c r="B476" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C476" s="0" t="s">
         <v>196</v>
@@ -18241,7 +18241,7 @@
         <v>193</v>
       </c>
       <c r="B477" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C477" s="0" t="s">
         <v>196</v>
@@ -18277,7 +18277,7 @@
         <v>193</v>
       </c>
       <c r="B478" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C478" s="0" t="s">
         <v>195</v>
@@ -18313,7 +18313,7 @@
         <v>193</v>
       </c>
       <c r="B479" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C479" s="0" t="s">
         <v>196</v>
@@ -18348,7 +18348,7 @@
         <v>193</v>
       </c>
       <c r="B480" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C480" s="0" t="s">
         <v>195</v>
@@ -18383,7 +18383,7 @@
         <v>193</v>
       </c>
       <c r="B481" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C481" s="0" t="s">
         <v>194</v>
@@ -18418,7 +18418,7 @@
         <v>198</v>
       </c>
       <c r="B482" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C482" s="0" t="s">
         <v>199</v>
@@ -18457,7 +18457,7 @@
         <v>198</v>
       </c>
       <c r="B483" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C483" s="0" t="s">
         <v>142</v>
@@ -18496,7 +18496,7 @@
         <v>198</v>
       </c>
       <c r="B484" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C484" s="0" t="s">
         <v>200</v>
@@ -18529,7 +18529,7 @@
         <v>198</v>
       </c>
       <c r="B485" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C485" s="0" t="s">
         <v>201</v>
@@ -18562,7 +18562,7 @@
         <v>198</v>
       </c>
       <c r="B486" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D486" s="0" t="s">
         <v>15</v>
@@ -18598,7 +18598,7 @@
         <v>198</v>
       </c>
       <c r="B487" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D487" s="0" t="s">
         <v>29</v>
@@ -18634,7 +18634,7 @@
         <v>198</v>
       </c>
       <c r="B488" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C488" s="0" t="s">
         <v>142</v>
@@ -18673,7 +18673,7 @@
         <v>198</v>
       </c>
       <c r="B489" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C489" s="0" t="s">
         <v>200</v>
@@ -18709,7 +18709,7 @@
         <v>198</v>
       </c>
       <c r="B490" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C490" s="0" t="s">
         <v>201</v>
@@ -18745,7 +18745,7 @@
         <v>198</v>
       </c>
       <c r="B491" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C491" s="0" t="s">
         <v>201</v>
@@ -18781,7 +18781,7 @@
         <v>198</v>
       </c>
       <c r="B492" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C492" s="0" t="s">
         <v>200</v>
@@ -18817,7 +18817,7 @@
         <v>198</v>
       </c>
       <c r="B493" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C493" s="0" t="s">
         <v>201</v>
@@ -18852,7 +18852,7 @@
         <v>198</v>
       </c>
       <c r="B494" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C494" s="0" t="s">
         <v>200</v>
@@ -18887,7 +18887,7 @@
         <v>198</v>
       </c>
       <c r="B495" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C495" s="0" t="s">
         <v>199</v>
@@ -18922,7 +18922,7 @@
         <v>198</v>
       </c>
       <c r="B496" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C496" s="0" t="s">
         <v>199</v>
@@ -18960,7 +18960,7 @@
         <v>198</v>
       </c>
       <c r="B497" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C497" s="0" t="s">
         <v>142</v>
@@ -18998,7 +18998,7 @@
         <v>198</v>
       </c>
       <c r="B498" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C498" s="0" t="s">
         <v>200</v>
@@ -19031,7 +19031,7 @@
         <v>198</v>
       </c>
       <c r="B499" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C499" s="0" t="s">
         <v>201</v>
@@ -19064,7 +19064,7 @@
         <v>198</v>
       </c>
       <c r="B500" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D500" s="0" t="s">
         <v>15</v>
@@ -19099,7 +19099,7 @@
         <v>198</v>
       </c>
       <c r="B501" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D501" s="0" t="s">
         <v>29</v>
@@ -19135,7 +19135,7 @@
         <v>198</v>
       </c>
       <c r="B502" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C502" s="0" t="s">
         <v>142</v>
@@ -19174,7 +19174,7 @@
         <v>198</v>
       </c>
       <c r="B503" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C503" s="0" t="s">
         <v>200</v>
@@ -19210,7 +19210,7 @@
         <v>198</v>
       </c>
       <c r="B504" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C504" s="0" t="s">
         <v>201</v>
@@ -19246,7 +19246,7 @@
         <v>198</v>
       </c>
       <c r="B505" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C505" s="0" t="s">
         <v>201</v>
@@ -19282,7 +19282,7 @@
         <v>198</v>
       </c>
       <c r="B506" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C506" s="0" t="s">
         <v>200</v>
@@ -19318,7 +19318,7 @@
         <v>198</v>
       </c>
       <c r="B507" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C507" s="0" t="s">
         <v>201</v>
@@ -19353,7 +19353,7 @@
         <v>198</v>
       </c>
       <c r="B508" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C508" s="0" t="s">
         <v>200</v>
@@ -19388,7 +19388,7 @@
         <v>198</v>
       </c>
       <c r="B509" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C509" s="0" t="s">
         <v>199</v>

</xml_diff>